<commit_message>
some changes for add scripts
</commit_message>
<xml_diff>
--- a/CURA DATAS/Cura_LOGIN_DATA.xlsx
+++ b/CURA DATAS/Cura_LOGIN_DATA.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="checkpoint" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -32,6 +33,18 @@
   </si>
   <si>
     <t xml:space="preserve">ThisIsNotAPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURA Healthcare Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make Appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appointment Confirmation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History</t>
   </si>
 </sst>
 </file>
@@ -41,7 +54,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -62,11 +75,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,7 +119,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -120,8 +128,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -249,8 +261,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F2:F3 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -283,4 +295,67 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>